<commit_message>
Adding Self service user testcases into Logixal QA box 2 env
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\LogixalQABox2\ALL_PAGES\END_TO_END\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366F97CC-9187-46DD-A781-FFDA3F612653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC32_Verify_store_location" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>TestCase</t>
   </si>
@@ -165,12 +171,21 @@
   </si>
   <si>
     <t>EnableCertificate_GoTOPage</t>
+  </si>
+  <si>
+    <t>CLEAR_TEXT</t>
+  </si>
+  <si>
+    <t>ContactUsEmail</t>
+  </si>
+  <si>
+    <t>kaman_automation_sanity_tc32@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -228,13 +243,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,11 +598,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -814,25 +832,23 @@
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>25</v>
@@ -845,57 +861,65 @@
         <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
       <c r="B22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
       <c r="B24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5">
@@ -904,12 +928,71 @@
         <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3"/>
+      <c r="B26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3"/>
+      <c r="B27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3"/>
+      <c r="B29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -919,17 +1002,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1042,6 +1125,22 @@
       </c>
       <c r="B14" s="3" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1050,21 +1149,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1261,24 +1345,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1295,4 +1377,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update TC32 : Logixal QA box 2 env
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\LogixalQABox2\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366F97CC-9187-46DD-A781-FFDA3F612653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1907DD87-45D5-463F-B729-7E5086CC6EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>TestCase</t>
   </si>
@@ -173,10 +173,10 @@
     <t>EnableCertificate_GoTOPage</t>
   </si>
   <si>
+    <t>ContactUsEmail</t>
+  </si>
+  <si>
     <t>CLEAR_TEXT</t>
-  </si>
-  <si>
-    <t>ContactUsEmail</t>
   </si>
   <si>
     <t>kaman_automation_sanity_tc32@yopmail.com</t>
@@ -599,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -832,23 +832,25 @@
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>25</v>
@@ -861,57 +863,55 @@
         <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
@@ -925,74 +925,52 @@
     <row r="25" spans="1:5">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3"/>
       <c r="B26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="3"/>
-      <c r="B29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="3"/>
-      <c r="B30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1003,16 +981,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B12" sqref="B12:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1129,18 +1107,10 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="3" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1149,6 +1119,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1345,15 +1324,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1361,6 +1331,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1379,14 +1357,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>

</xml_diff>